<commit_message>
fixed compare other robot v2
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/TM5_700_tested_state_original_design_case2.xlsx
+++ b/dynamics/src/dynamics/xlsx/TM5_700_tested_state_original_design_case2.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,10 +428,16 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="C1" t="n">
-        <v>0.02062288336709792</v>
+        <v>0.04146758932281736</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>202.0454051677636</v>
       </c>
     </row>
     <row r="2">
@@ -441,10 +447,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01670443718583834</v>
+        <v>0.01989412373158344</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>183.0146123922239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>